<commit_message>
adding changes to support spanish documennts and pdf docs
</commit_message>
<xml_diff>
--- a/samples/contract-compliance-analysis/back-end/guidelines/guidelines_example.xlsx
+++ b/samples/contract-compliance-analysis/back-end/guidelines/guidelines_example.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gdalves/dev/aee/ifood/anonymized/ifood-backend-anonym-draft/guidelines/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luisff/Documents/workspace/generative-ai-cdk-constructs-samples/samples/contract-compliance-analysis/back-end/guidelines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FAEB3C-AD55-144B-9ACC-A632C993EF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5B6CA2-7C5E-EF40-B177-19B197B4B3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37060" yWindow="2680" windowWidth="40460" windowHeight="24140" xr2:uid="{FD2DBF6C-2FF1-CD4F-A391-81725205B6E0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{FD2DBF6C-2FF1-CD4F-A391-81725205B6E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Taxonomy" sheetId="1" r:id="rId1"/>
     <sheet name="Examples" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Taxonomy!$E$1:$H$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Taxonomy!$E$1:$H$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="256">
   <si>
     <t>Id</t>
   </si>
@@ -693,250 +693,6 @@
   </si>
   <si>
     <t>Example</t>
-  </si>
-  <si>
-    <t>Does the clause specify that the Service Provider must perform the services in a professional manner?
-Does the clause require the Service Provider to perform the services in a timely manner?
-Does the clause state that the Service Provider must perform the services in a workmanlike manner?
-Does the clause indicate that the services must be performed consistent with industry standards?
-Does the clause specify that the services must be performed consistent with best practices?
-Does the clause require the Service Provider to perform the services in accordance with the specifications set forth in the Statement of Work?
-Does the clause require the Service Provider to perform the services in accordance with the requirements set forth in the Statement of Work?</t>
-  </si>
-  <si>
-    <t>Does the clause specify that the Service Provider is responsible for providing certain deliverables?
-Does the clause indicate that the deliverables to be provided are specified in a Statement of Work?
-Does the clause state that the Service Provider must provide the deliverables in accordance with agreed-upon timelines?
-Does the clause state that the Service Provider must provide the deliverables in accordance with agreed-upon milestones?</t>
-  </si>
-  <si>
-    <t>Does the clause give the company the right to review and test deliverables?
-Does the clause state that the company can reject deliverables that fail to meet acceptance criteria?
-Does the clause require the service provider to remedy deficiencies in rejected deliverables at no additional cost to the company?
-Does the clause mention acceptance criteria being set forth in a Statement of Work?</t>
-  </si>
-  <si>
-    <t>Does the clause mention that the Service Provider shall cooperate with the Company?
-Does the clause mention that the Service Provider shall cooperate with any third-party service providers?
-Does the clause mention that the cooperation is to ensure a smooth transition of the Services?
-Does the clause mention that the cooperation is to ensure a smooth implementation of the Services?
-Does the clause mention that the cooperation includes providing necessary training?
-Does the clause mention that the cooperation includes providing necessary documentation?
-Does the clause mention that the cooperation includes providing necessary knowledge transfer?</t>
-  </si>
-  <si>
-    <t>Does the clause specify when the agreement commences?
-Does the clause mention that the agreement will continue for a specified term?
-Does the clause indicate that the agreement can be terminated earlier under certain conditions?
-Does the clause refer to a separate document called "Statement of Work" for specifying the term of the agreement?</t>
-  </si>
-  <si>
-    <t>Does the clause mention the possibility of renewing or extending the agreement?
-Does the clause state that renewal or extension requires mutual written agreement between the parties?
-Does the clause indicate that renewal or extension would be subject to the same terms and conditions as the current agreement?
-Does the clause allow for the possibility of different terms and conditions upon renewal or extension, if agreed upon by the parties?</t>
-  </si>
-  <si>
-    <t>Does the clause specify that the company will pay fees to the service provider?
-Does the clause mention a statement of work that specifies the fees to be paid?
-Does the clause indicate that the payment schedule is set forth in the statement of work?
-Does the clause state that the company will pay the fees in accordance with the payment schedule?</t>
-  </si>
-  <si>
-    <t>Does the clause specify that the Service Provider shall submit invoices to the Company?
-Does the clause mention that the invoices should be submitted in accordance with invoicing instructions provided in a Statement of Work?
-Does the clause state that the Company shall pay undisputed invoices?
-Does the clause specify a time period within which the Company shall pay undisputed invoices after receipt?</t>
-  </si>
-  <si>
-    <t>Does the clause specify that the Service Provider is responsible for all expenses incurred in performing the Services, unless otherwise stated in the Statement of Work?
-Does the clause state that if expense reimbursement is permitted, the Service Provider must provide detailed documentation and receipts for all reimbursable expenses?
-Does the clause mention that the Company shall reimburse the Service Provider's expenses in accordance with its expense reimbursement policies, if reimbursement is permitted?</t>
-  </si>
-  <si>
-    <t>Does the clause state that each party is responsible for paying applicable taxes, fees, or other charges imposed by any governmental authority in connection with the performance of the agreement?
-Does the clause specify that if the Service Provider is required to collect or remit any taxes on behalf of the Company, the Service Provider shall separately state such taxes on its invoices?
-Does the clause indicate that the Company shall pay any taxes separately stated by the Service Provider on invoices, in addition to the fees for the Services?</t>
-  </si>
-  <si>
-    <t>Does the clause mention a Service Provider?
-Does the clause mention a Company?
-Does the clause mention service levels or performance standards?
-Does the clause mention that the Company is entitled to service credits or service level rebates if the Service Provider fails to meet the specified service levels or performance standards?
-Does the clause specify that the service credits or service level rebates are set forth in the Statement of Work?</t>
-  </si>
-  <si>
-    <t>Does the clause specify that each party retains ownership of their pre-existing intellectual property rights?
-Does the clause mention that pre-existing intellectual property rights include patents, copyrights, trademarks, and trade secrets?
-Does the clause state that any new intellectual property developed during the performance of services will be owned by the company?
-Does the clause allow for exceptions to the ownership of new intellectual property, if specified in a separate Statement of Work?</t>
-  </si>
-  <si>
-    <t>Does the clause define what constitutes Confidential Information?
-Does the clause specify that Confidential Information excludes information that is publicly available through no fault of the receiving party?
-Does the clause specify that Confidential Information excludes information rightfully received from a third party without breach of confidentiality?
-Does the clause specify that Confidential Information excludes information independently developed by the receiving party without using the disclosing party's Confidential Information?
-Does the clause specify that Confidential Information excludes information already known to the receiving party prior to disclosure, as evidenced by written records?</t>
-  </si>
-  <si>
-    <t>Does the clause state that the Service Provider has the necessary skills, qualifications, and expertise to perform the Services?
-Does the clause state that the Services will be performed in a professional and workmanlike manner?
-Does the clause state that the Deliverables will conform to the specifications and requirements set forth in the Statement of Work?
-Does the clause state that the Deliverables will not infringe upon any third-party intellectual property rights?</t>
-  </si>
-  <si>
-    <t>Does the clause require the Service Provider to indemnify the Company?
-Does the clause require the Service Provider to defend the Company?
-Does the clause require the Service Provider to hold the Company harmless?
-Does the clause cover the Company's affiliates in addition to the Company itself?
-Does the clause cover the officers, directors, employees, and agents of the Company and its affiliates?
-Does the clause cover claims, demands, suits, actions, proceedings, losses, liabilities, damages, costs, and expenses (including reasonable attorneys' fees)?
-Does the clause cover situations arising out of or relating to a breach of the Agreement by the Service Provider?
-Does the clause cover situations arising out of or relating to any negligent or willful act or omission by the Service Provider or its employees, agents, or subcontractors in the performance of the Services?
-Does the clause cover situations arising out of or relating to any allegation that the Deliverables or Services infringe upon any third-party intellectual property rights?</t>
-  </si>
-  <si>
-    <t>Does the clause limit the liability of both parties for certain types of damages?
-Does the clause exclude liability for indirect, incidental, special, punitive, or consequential damages?
-Does the clause provide examples of the types of damages excluded, such as lost profits, lost revenue, or business interruption?
-Does the clause make an exception for claims arising out of a party's indemnification obligations, gross negligence, or willful misconduct?
-Does the clause state that the limitation of liability applies even if a party was advised of the possibility of such damages?</t>
-  </si>
-  <si>
-    <t>Does the clause mention that neither party is liable for delays or failures to perform obligations due to causes beyond their reasonable control?
-Does the clause provide examples of such causes, including acts of God, acts of civil or military authority, fires, floods, earthquakes, riots, wars, terrorist acts, epidemics, or governmental restrictions?
-Does the clause refer to these causes collectively as a "Force Majeure Event"?
-Does the clause require the affected party to promptly notify the other party in the event of a Force Majeure Event?
-Does the clause state that the parties shall work together in good faith to mitigate the effects of the Force Majeure Event?
-Does the clause allow for the possibility of amending or terminating the agreement if necessary due to a Force Majeure Event?</t>
-  </si>
-  <si>
-    <t>Does the clause state that each party shall comply with all applicable anti-corruption laws?
-Does the clause prohibit engaging in any form of bribery?
-Does the clause prohibit engaging in any form of kickbacks?
-Does the clause prohibit engaging in any other form of corrupt practices in connection with the agreement?
-Does the clause mention the U.S. Foreign Corrupt Practices Act?
-Does the clause mention the UK Bribery Act?</t>
-  </si>
-  <si>
-    <t>Does the clause mention that the parties must comply with applicable laws and regulations?
-Does the clause specify that the laws and regulations relate to corporate social responsibility?
-Does the clause include environmental protection as one of the areas covered by corporate social responsibility?
-Does the clause include labor practices as one of the areas covered by corporate social responsibility?
-Does the clause include human rights as one of the areas covered by corporate social responsibility?
-Does the clause indicate that the listed areas (environmental protection, labor practices, and human rights) are not an exhaustive list of areas covered by corporate social responsibility?</t>
-  </si>
-  <si>
-    <t>Does the clause require the Service Provider to assign personnel to perform the Services?
-Does the clause specify that the personnel assigned must be qualified and experienced?
-Does the clause require the Service Provider to allocate sufficient resources to meet the requirements and timelines set forth in the Statement of Work?
-Does the clause mention a Statement of Work that sets forth requirements and timelines?</t>
-  </si>
-  <si>
-    <t>Does the clause mention that the Company has the right to object to the performance or conduct of the Service Provider's personnel?
-Does the clause state that if the Company objects, the Service Provider must replace the personnel in question?
-Does the clause specify that the replacements for the personnel must be qualified and experienced?
-Does the clause require that the replacements must be acceptable to the Company?
-Does the clause indicate that the Service Provider must replace the personnel promptly if the Company objects?</t>
-  </si>
-  <si>
-    <t>Does the clause require the Service Provider to ensure that all of its employees, agents, and subcontractors assigned to perform Services under the Agreement have successfully completed background checks?
-Does the clause require the Service Provider to ensure that all of its employees, agents, and subcontractors assigned to perform Services under the Agreement have obtained any necessary security clearances?
-Does the clause specify that the background checks and security clearances are required by the Company or applicable laws and regulations?
-Does the clause apply to the Service Provider's employees, agents, and subcontractors assigned to perform Services under the Agreement?
-Does the clause relate to the Service Provider's obligations regarding background checks and security clearances for its personnel assigned to perform Services under the Agreement?</t>
-  </si>
-  <si>
-    <t>Does the clause prohibit either party from assigning or transferring the agreement without the other party's consent?
-Does the clause require the other party's consent to be in written form?
-Does the clause state that the other party's consent should not be unreasonably withheld or delayed?
-Does the clause apply the restriction on assignment or transfer to both parties equally?
-Does the clause apply the restriction to both the assignment/transfer of the agreement itself and the assignment/transfer of rights or obligations under the agreement?</t>
-  </si>
-  <si>
-    <t>Does the clause allow the Service Provider to engage subcontractors to perform certain Services?
-Does the clause state that the Service Provider remains responsible for the performance of any subcontractors engaged?
-Does the clause require that any subcontractors engaged by the Service Provider comply with the terms and conditions of the Agreement?</t>
-  </si>
-  <si>
-    <t>Does the clause specify two parties?
-Does the clause prohibit certain actions by the parties during the term of the agreement?
-Does the clause prohibit certain actions by the parties for a period after the term of the agreement?
-Does the clause specify a duration for the period after the term of the agreement?
-Does the clause prohibit circumventing or attempting to circumvent the other party's business relationships?
-Does the clause prohibit circumventing or attempting to circumvent the other party's contractual arrangements with third parties?</t>
-  </si>
-  <si>
-    <t>Does the clause mention the right of the company to audit the service provider's records and facilities?
-Does the clause specify that the audit is for verifying compliance with the agreement?
-Does the clause state that the company must provide reasonable notice before conducting the audit?
-Does the clause indicate that the audit can only be conducted during regular business hours?</t>
-  </si>
-  <si>
-    <t>Does the clause mention the parties being unable to resolve a dispute through negotiations?
-Does the clause specify a time period (in days) for the parties to attempt negotiations before proceeding further?
-Does the clause mention the parties submitting the dispute to non-binding mediation if negotiations fail?
-Does the clause reference the rules of a specific mediation service provider?</t>
-  </si>
-  <si>
-    <t>Does the clause mention mediation as a step before pursuing binding arbitration or litigation?
-Does the clause state that binding arbitration can be pursued if the dispute cannot be resolved through mediation?
-Does the clause specify that the binding arbitration should be in accordance with the rules of an Arbitration Service Provider?
-Does the clause indicate that litigation in a court of competent jurisdiction can be pursued if the parties mutually agree?
-Does the clause mention that either party may pursue binding arbitration or litigation?</t>
-  </si>
-  <si>
-    <t>Does the clause specify that all communications under the agreement must be in writing?
-Does the clause list the acceptable methods for delivering written communications?
-Does the clause include hand delivery with written confirmation of receipt as an acceptable method?
-Does the clause include delivery by a nationally recognized overnight courier (with receipt requested) as an acceptable method?
-Does the clause include email delivery as an acceptable method?
-Does the clause specify conditions for when an email is considered duly delivered based on the time it was sent?
-Does the clause include certified or registered mail (return receipt requested) as an acceptable method?
-Does the clause specify a timeframe for when a communication sent by certified or registered mail is considered duly delivered?</t>
-  </si>
-  <si>
-    <t>Does the clause address the situation where one or more provisions of the agreement are deemed invalid, illegal, or unenforceable?
-Does the clause state that the validity, legality, and enforceability of the remaining provisions will not be affected or impaired if one or more provisions are deemed invalid, illegal, or unenforceable?
-Does the clause use the term "Agreement" to refer to the contract or agreement being discussed?
-Does the clause avoid making any deductions, proposing premises, making generalizations, or implying/deducing implicit content?</t>
-  </si>
-  <si>
-    <t>Does the clause mention that no waiver of a breach is considered a waiver of any other breach?
-Does the clause state that a waiver is only effective if made in writing?
-Does the clause specify that a waiver must be signed by an authorized representative of the waiving party?
-Does the clause indicate that the waiver applies to both parties?
-Does the clause mention that the waiver applies to any provision of the agreement?</t>
-  </si>
-  <si>
-    <t>Does the clause prohibit one party from using the other party's name without prior written consent?
-Does the clause prohibit one party from using the other party's logo without prior written consent?
-Does the clause prohibit one party from using the other party's trademarks without prior written consent?
-Does the clause prohibit the use of the other party's name, logo, or trademarks in publicity materials without prior written consent?
-Does the clause prohibit the use of the other party's name, logo, or trademarks in advertising materials without prior written consent?
-Does the clause prohibit the use of the other party's name, logo, or trademarks in marketing materials without prior written consent?
-Does the clause apply the prohibition of using the other party's name, logo, or trademarks without prior written consent to both parties?</t>
-  </si>
-  <si>
-    <t>Does the clause specify that the Service Provider must ensure that the fees and terms offered to the Company are at least as favorable as those offered to any other customer or nation for similar services?
-Is it stated in the clause that the requirement for the Service Provider to offer fees and terms at least as favorable as those offered to others is conditional on it being specified in the Statement of Work?
-Does the clause mention both fees and terms that the Service Provider must ensure are at least as favorable as those offered to others?
-Is the Company explicitly mentioned as the party to whom the Service Provider must offer fees and terms that are at least as favorable as those offered to others?
-Does the clause specify that the requirement applies to fees and terms offered for similar services, without further qualification?</t>
-  </si>
-  <si>
-    <t>Does the clause mention that the parties involved are required to cooperate with each other?
-Does the clause state that the parties involved are required to provide assistance to each other?
-Does the clause specify that the cooperation and assistance are in connection with the performance of obligations under the agreement?
-Does the clause indicate that the cooperation and assistance are reasonable?
-Does the clause apply the requirement of cooperation and assistance to both parties involved?</t>
-  </si>
-  <si>
-    <t>Does the clause explicitly state that the relationship between the parties is that of independent contractors?
-Does the clause explicitly deny the existence of an employer-employee relationship between the parties?
-Does the clause explicitly deny the existence of a partnership between the parties?
-Does the clause explicitly deny the existence of a joint venture between the parties?
-Does the clause explicitly deny the existence of an agency relationship between the parties?</t>
   </si>
   <si>
     <t>a. Term: This Agreement shall commence on the Effective Date and shall continue for the term specified in the Statement of Work, unless earlier terminated in accordance with this Section.
@@ -954,32 +710,6 @@
     <t>This Agreement shall be governed by and construed in accordance with the laws of [Governing Jurisdiction], without regard to its conflict of laws principles. The Parties hereby submit to the exclusive jurisdiction of the courts located in [Jurisdiction] for any legal proceedings arising out of or relating to this Agreement.</t>
   </si>
   <si>
-    <t>Does the clause specify the governing law for the agreement?
-Does the clause mention that the agreement shall be construed in accordance with the laws of a specific jurisdiction?
-Does the clause state that the parties submit to the exclusive jurisdiction of courts located in a specific location for any legal proceedings related to the agreement?
-Does the clause disregard conflict of laws principles for the governing jurisdiction?</t>
-  </si>
-  <si>
-    <t>Does the clause require the receiving party to use at least reasonable care to protect the confidential information?
-Does the clause prohibit the receiving party from using the confidential information for any purpose other than performing obligations under the agreement?
-Does the clause allow the receiving party to disclose the confidential information to its employees, agents, or contractors who have a need to know and are bound by confidentiality obligations at least as protective as those set forth in the clause?</t>
-  </si>
-  <si>
-    <t>Does the clause mention that the services are to be provided on an exclusive basis if specified in the Statement of Work?
-Does the clause prohibit the Service Provider from providing similar services to third parties during the term of the Agreement?
-Does the clause specify that providing similar services to third parties requires prior written consent from the Company?</t>
-  </si>
-  <si>
-    <t>Does the clause mention that it applies in case of any dispute or disagreement related to the agreement?
-Does the clause state that the parties involved must first try to resolve the dispute?
-Does the clause specify that the parties must attempt to resolve the dispute through good faith negotiations?</t>
-  </si>
-  <si>
-    <t>Does the clause prohibit both parties from making disparaging or defamatory statements during the term of the agreement and for some period after its termination?
-Does the clause cover both written and oral disparaging or defamatory statements?
-Does the clause prohibit disparaging or defamatory statements about the other party, its products, services, employees, or business practices?</t>
-  </si>
-  <si>
     <t>high</t>
   </si>
   <si>
@@ -992,26 +722,115 @@
     <t>Impact</t>
   </si>
   <si>
-    <t>Does the contract clause state that the agreement, together with the Statement of Work and any other exhibits or attachments, constitutes the entire agreement between the Parties with respect to the subject matter?
-Does the contract clause state that the agreement supersedes all prior agreements, understandings, and negotiations, both written and oral, between the Parties with respect to the subject matter of the agreement?
-Does the contract clause state that the agreement may be amended or modified only by a written instrument duly executed by authorized representatives of both Parties?</t>
+    <t>Esta sección establece la identidad legal de los participantes en el contrato. Debe incluir información completa y precisa del club deportivo (incluyendo su registro fiscal, domicilio legal y representante autorizado) así como los datos personales del jugador (identificación oficial, domicilio, nacionalidad). La precisión en esta sección es fundamental para la validez legal del contrato.</t>
+  </si>
+  <si>
+    <t>Identificación de las partes</t>
+  </si>
+  <si>
+    <t>¿Están correctamente especificados los datos fiscales del club?
+¿Se incluye la documentación que acredita al representante legal del club?
+¿Los datos personales del jugador están completos y verificados?</t>
+  </si>
+  <si>
+    <t>Objeto y Duración</t>
+  </si>
+  <si>
+    <t>Define el propósito específico del contrato y su marco temporal. Debe establecer claramente las funciones del jugador como profesional, las categorías en las que participará, y el período exacto de vigencia del contrato. Esta sección es crucial para establecer el alcance de la relación laboral deportiva.</t>
+  </si>
+  <si>
+    <t>¿Está claramente definido el rol y las funciones del jugador?
+¿Las fechas de inicio y término están claramente establecidas?</t>
+  </si>
+  <si>
+    <t>Remuneración</t>
+  </si>
+  <si>
+    <t>Detalla todos los aspectos económicos del contrato, incluyendo salario base, bonificaciones, primas y cualquier otro beneficio económico. Debe especificar montos, periodicidad de pagos, condiciones para bonos y método de pago. Esta sección es fundamental para evitar disputas económicas futuras.</t>
+  </si>
+  <si>
+    <t>¿Están detallados todos los componentes del salario?
+¿Los bonos por rendimiento tienen métricas claras de medición?</t>
+  </si>
+  <si>
+    <t>Obligaciones del jugador</t>
+  </si>
+  <si>
+    <t>Establece los deberes y responsabilidades específicos del jugador, incluyendo requisitos de rendimiento, conducta profesional, participación en entrenamientos y partidos, y cumplimiento de normas del club. Define las expectativas específicas que el club tiene sobre el desempeño y comportamiento del jugador.</t>
+  </si>
+  <si>
+    <t>¿Las obligaciones de rendimiento físico son medibles?
+¿Están definidas las consecuencias del incumplimiento?</t>
+  </si>
+  <si>
+    <t>Obligaciones del Club</t>
+  </si>
+  <si>
+    <t>Define las responsabilidades del club hacia el jugador, incluyendo provisión de instalaciones, equipamiento, servicios médicos, y cumplimiento de obligaciones financieras. Esta sección garantiza que el club proporcione el entorno y recursos necesarios para el desempeño profesional del jugador.</t>
+  </si>
+  <si>
+    <t>¿Están especificados los servicios médicos y seguros?
+¿Se detallan las instalaciones y equipamiento a proporcionar?</t>
+  </si>
+  <si>
+    <t>Derechos de imagen</t>
+  </si>
+  <si>
+    <t>Regula el uso y explotación de la imagen del jugador por parte del club. Debe especificar los términos de uso, distribución de beneficios económicos, y limitaciones. Esta sección es crucial en la era moderna del fútbol donde los derechos de imagen tienen un valor significativo.</t>
+  </si>
+  <si>
+    <t>¿Está clara la distribución de ingresos por derechos de imagen?
+¿Se especifican los límites de uso de imagen?</t>
+  </si>
+  <si>
+    <t>Transferencias</t>
+  </si>
+  <si>
+    <t>Establece las condiciones bajo las cuales el jugador puede ser transferido a otro club, incluyendo los derechos económicos, proceso de negociación y distribución de beneficios. Esta sección es fundamental para proteger los intereses tanto del club como del jugador en caso de una transferencia.</t>
+  </si>
+  <si>
+    <t>¿Está clara la distribución de derechos económicos?
+¿Se especifica el proceso de negociación de transferencias?</t>
+  </si>
+  <si>
+    <t>Causas de rescisión</t>
+  </si>
+  <si>
+    <t>Define las circunstancias bajo las cuales el contrato puede ser terminado anticipadamente por cualquiera de las partes. Debe incluir causales específicas, proceso de notificación y consecuencias económicas de la rescisión.</t>
+  </si>
+  <si>
+    <t>¿Están definidas todas las causales de rescisión?
+¿Se especifica el proceso de notificación de rescisión?</t>
+  </si>
+  <si>
+    <t>Confidencialidad</t>
+  </si>
+  <si>
+    <t>Establece las obligaciones de confidencialidad de ambas partes respecto a la información sensible del contrato y operaciones del club. Define qué información debe mantenerse confidencial y las consecuencias de su divulgación.</t>
+  </si>
+  <si>
+    <t>¿Están definidos los términos de confidencialidad?
+¿Se especifican las penalizaciones por incumplimiento?</t>
+  </si>
+  <si>
+    <t>Jurisdicción</t>
+  </si>
+  <si>
+    <t>Determina la jurisdicción legal aplicable y los mecanismos de resolución de disputas. Debe alinearse con los reglamentos de la Federación Mexicana de Fútbol y establecer claramente el proceso para resolver conflictos.</t>
+  </si>
+  <si>
+    <t>¿Está claramente definida la jurisdicción aplicable?
+¿Se especifica el proceso de resolución de conflictos?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1037,16 +856,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1372,17 +1188,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2763079-711B-9546-BF78-5DCA270CA6BA}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.1640625" customWidth="1"/>
     <col min="2" max="2" width="44.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="143" customWidth="1"/>
+    <col min="3" max="3" width="255.83203125" customWidth="1"/>
+    <col min="4" max="4" width="85.1640625" customWidth="1"/>
     <col min="5" max="5" width="27.6640625" customWidth="1"/>
     <col min="6" max="6" width="175.1640625" customWidth="1"/>
   </cols>
@@ -1398,7 +1215,7 @@
         <v>213</v>
       </c>
       <c r="E1" t="s">
-        <v>265</v>
+        <v>225</v>
       </c>
       <c r="F1" t="s">
         <v>216</v>
@@ -1410,21 +1227,21 @@
         <v>215</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="118" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>227</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>226</v>
       </c>
       <c r="E2" t="s">
-        <v>263</v>
+        <v>222</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1432,16 +1249,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>229</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>230</v>
       </c>
       <c r="E3" t="s">
-        <v>262</v>
+        <v>222</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1449,16 +1266,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>232</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>233</v>
       </c>
       <c r="E4" t="s">
-        <v>263</v>
+        <v>223</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>220</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1466,16 +1283,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>235</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>236</v>
       </c>
       <c r="E5" t="s">
-        <v>263</v>
-      </c>
-      <c r="F5" t="s">
-        <v>221</v>
+        <v>223</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1483,16 +1300,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
+      </c>
+      <c r="C6" t="s">
+        <v>239</v>
       </c>
       <c r="E6" t="s">
-        <v>262</v>
-      </c>
-      <c r="F6" t="s">
         <v>222</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1500,16 +1317,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>241</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>242</v>
       </c>
       <c r="E7" t="s">
-        <v>263</v>
-      </c>
-      <c r="F7" t="s">
-        <v>223</v>
+        <v>224</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1517,16 +1334,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>244</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>245</v>
       </c>
       <c r="E8" t="s">
-        <v>262</v>
-      </c>
-      <c r="F8" t="s">
-        <v>224</v>
+        <v>222</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1534,16 +1351,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>248</v>
       </c>
       <c r="E9" t="s">
-        <v>263</v>
-      </c>
-      <c r="F9" t="s">
-        <v>225</v>
+        <v>223</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1551,16 +1368,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>250</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>251</v>
       </c>
       <c r="E10" t="s">
-        <v>263</v>
-      </c>
-      <c r="F10" t="s">
-        <v>226</v>
+        <v>223</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1568,543 +1385,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>253</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>254</v>
       </c>
       <c r="E11" t="s">
-        <v>263</v>
-      </c>
-      <c r="F11" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" t="s">
-        <v>262</v>
-      </c>
-      <c r="F12" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" t="s">
-        <v>263</v>
-      </c>
-      <c r="F13" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" t="s">
-        <v>262</v>
-      </c>
-      <c r="F14" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" t="s">
-        <v>262</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" t="s">
-        <v>263</v>
-      </c>
-      <c r="F16" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E17" t="s">
-        <v>263</v>
-      </c>
-      <c r="F17" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" t="s">
-        <v>262</v>
-      </c>
-      <c r="F18" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" t="s">
-        <v>263</v>
-      </c>
-      <c r="F19" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" t="s">
-        <v>263</v>
-      </c>
-      <c r="F20" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" t="s">
-        <v>64</v>
-      </c>
-      <c r="E21" t="s">
-        <v>263</v>
-      </c>
-      <c r="F21" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" t="s">
-        <v>263</v>
-      </c>
-      <c r="F22" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" t="s">
-        <v>263</v>
-      </c>
-      <c r="F23" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" t="s">
-        <v>263</v>
-      </c>
-      <c r="F24" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" t="s">
-        <v>263</v>
-      </c>
-      <c r="F25" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" t="s">
-        <v>263</v>
-      </c>
-      <c r="F26" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" t="s">
-        <v>263</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" t="s">
-        <v>72</v>
-      </c>
-      <c r="E28" t="s">
-        <v>263</v>
-      </c>
-      <c r="F28" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" t="s">
-        <v>262</v>
-      </c>
-      <c r="F29" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" t="s">
-        <v>74</v>
-      </c>
-      <c r="E30" t="s">
-        <v>264</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" t="s">
-        <v>75</v>
-      </c>
-      <c r="E31" t="s">
-        <v>264</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" t="s">
-        <v>76</v>
-      </c>
-      <c r="E32" t="s">
-        <v>263</v>
-      </c>
-      <c r="F32" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" t="s">
-        <v>78</v>
-      </c>
-      <c r="E33" t="s">
-        <v>264</v>
-      </c>
-      <c r="F33" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" t="s">
-        <v>79</v>
-      </c>
-      <c r="E34" t="s">
-        <v>264</v>
-      </c>
-      <c r="F34" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" t="s">
-        <v>80</v>
-      </c>
-      <c r="E35" t="s">
-        <v>264</v>
-      </c>
-      <c r="F35" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" t="s">
-        <v>81</v>
-      </c>
-      <c r="E36" t="s">
-        <v>264</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" t="s">
-        <v>82</v>
-      </c>
-      <c r="E37" t="s">
-        <v>264</v>
-      </c>
-      <c r="F37" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" t="s">
-        <v>83</v>
-      </c>
-      <c r="E38" t="s">
-        <v>263</v>
-      </c>
-      <c r="F38" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" t="s">
-        <v>84</v>
-      </c>
-      <c r="E39" t="s">
-        <v>263</v>
-      </c>
-      <c r="F39" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
+        <v>223</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="C40" t="s">
-        <v>85</v>
-      </c>
-      <c r="E40" t="s">
-        <v>264</v>
-      </c>
-      <c r="F40" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41" t="s">
-        <v>43</v>
-      </c>
-      <c r="C41" t="s">
-        <v>183</v>
-      </c>
-      <c r="E41" t="s">
-        <v>263</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" t="s">
-        <v>256</v>
-      </c>
-      <c r="E42" t="s">
-        <v>262</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -2114,7 +1404,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E2:E42" xr:uid="{31D2C625-39C2-8E41-929F-C576EF816B93}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E2:E11" xr:uid="{31D2C625-39C2-8E41-929F-C576EF816B93}">
       <formula1>"low, medium, high"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2366,7 +1656,7 @@
         <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>253</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2492,7 +1782,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>254</v>
+        <v>219</v>
       </c>
       <c r="B33">
         <v>8</v>
@@ -3977,7 +3267,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="B168">
         <v>43</v>
@@ -3988,7 +3278,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="B169">
         <v>43</v>
@@ -3999,7 +3289,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="B170">
         <v>43</v>
@@ -4010,7 +3300,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="B171">
         <v>43</v>
@@ -4104,7 +3394,7 @@
         <v>45</v>
       </c>
       <c r="C179" t="s">
-        <v>256</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>